<commit_message>
Readme update and ViT reference added
</commit_message>
<xml_diff>
--- a/2 SIIM-FISABIO-RSNA COVID-19 Detection/MMDetection_Backbone_models.xlsx
+++ b/2 SIIM-FISABIO-RSNA COVID-19 Detection/MMDetection_Backbone_models.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Haenara.SHIN/Documents/2 Study (Python, Math)/99 Kaggle/2 SIIM-FISABIO-RSNA COVID-19 Detection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBE42E4-DFD8-8C44-8520-72989DC0432B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9852E664-5433-8E43-BE9D-2A0AF0305343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3940" yWindow="980" windowWidth="28300" windowHeight="16180" xr2:uid="{4D516184-E40F-A447-9234-7D680F371712}"/>
+    <workbookView xWindow="-29280" yWindow="860" windowWidth="28300" windowHeight="16180" xr2:uid="{4D516184-E40F-A447-9234-7D680F371712}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -391,13 +391,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.499984740745262"/>
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -777,7 +777,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -954,23 +954,23 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="2" customFormat="1">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:10" s="11" customFormat="1">
+      <c r="A8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="11">
         <v>9.9</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="11">
         <v>47.4</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="12" t="s">
         <v>33</v>
       </c>
     </row>
@@ -994,23 +994,23 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="9" customFormat="1">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:10" s="2" customFormat="1">
+      <c r="A10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="2">
         <v>47.1</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1154,23 +1154,23 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="11" customFormat="1">
-      <c r="A18" s="11" t="s">
+    <row r="18" spans="1:7" s="9" customFormat="1">
+      <c r="A18" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="9">
         <v>49.7</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G18" s="10" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>